<commit_message>
Power analysis; updates to 205pd
Started analysis based on the 204 with an architecture diagram and with an smath document. Copied over manually changes from the 205 branch and started updating the schematic with USB PD capabilities. Only added decoy USB PD chip (CH224K), still need to fix power supplies.
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra/Manufacturing Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxe-205/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E1BBE-202C-3544-BD2A-66A15896674A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2B2FE-58A6-8D4F-9695-61E1868ABFF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33760" windowHeight="25840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28320" windowHeight="25240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="172">
   <si>
     <t>Qty</t>
   </si>
@@ -38,9 +38,6 @@
     <t>PARTNO</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
     <t>C1, C7, C9, C19, C20, C29, C33, C42, C52</t>
   </si>
   <si>
@@ -203,37 +200,13 @@
     <t>C3216X5R0J107M160AB</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SS310</t>
-  </si>
-  <si>
-    <t>SK310A-LTPMSCT-ND</t>
-  </si>
-  <si>
-    <t>SK310A-LTP</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>54-00164</t>
-  </si>
-  <si>
-    <t>839-54-00164CT-ND</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>455-B2B-XH-A-ND</t>
-  </si>
-  <si>
-    <t>B2B-XH-A</t>
+    <t>PJ-036AH-SMT</t>
+  </si>
+  <si>
+    <t>CP-036AHPJTR-ND</t>
   </si>
   <si>
     <t>J4</t>
@@ -260,6 +233,15 @@
     <t>USB4105-GF-A</t>
   </si>
   <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>S5596-ND</t>
+  </si>
+  <si>
+    <t>NPTC041KFXC-RC</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -554,13 +536,7 @@
     <t>SC32S-7PF20PPM</t>
   </si>
   <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>S5596-ND</t>
-  </si>
-  <si>
-    <t>NPTC041KFXC-RC</t>
+    <t>NOPE</t>
   </si>
 </sst>
 </file>
@@ -951,20 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,263 +955,260 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1244,13 +1216,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>65</v>
@@ -1261,16 +1233,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,16 +1250,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1295,118 +1267,118 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
         <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
         <v>86</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
         <v>90</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>99</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,16 +1386,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
         <v>102</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1431,16 +1403,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>107</v>
-      </c>
-      <c r="D28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1448,16 +1420,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="s">
         <v>110</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>111</v>
-      </c>
-      <c r="D29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,16 +1437,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
         <v>114</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>115</v>
-      </c>
-      <c r="D30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1482,16 +1454,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>119</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1499,50 +1471,50 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
         <v>122</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>123</v>
-      </c>
-      <c r="D32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s">
         <v>126</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
         <v>130</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>131</v>
-      </c>
-      <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1550,16 +1522,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" t="s">
         <v>134</v>
       </c>
-      <c r="C35" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" t="s">
-        <v>136</v>
-      </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1567,16 +1539,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" t="s">
         <v>138</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1584,16 +1556,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
         <v>141</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>142</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1601,16 +1573,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" t="s">
         <v>145</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>146</v>
-      </c>
-      <c r="D38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1618,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" t="s">
         <v>149</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>150</v>
-      </c>
-      <c r="D39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1635,16 +1607,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" t="s">
         <v>153</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>154</v>
-      </c>
-      <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1652,16 +1624,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
         <v>157</v>
       </c>
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1669,16 +1641,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1686,16 +1658,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" t="s">
         <v>164</v>
-      </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1703,16 +1675,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1720,44 +1689,16 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1767,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1795,10 +1736,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1806,10 +1747,10 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1817,10 +1758,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1828,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1839,10 +1780,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1850,10 +1791,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1861,10 +1802,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1872,10 +1813,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1883,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1894,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1905,10 +1846,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1916,10 +1857,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1927,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1938,10 +1879,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1949,10 +1890,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1960,10 +1901,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1971,10 +1912,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1982,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1993,76 +1934,76 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
         <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
         <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
         <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2070,10 +2011,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2081,10 +2022,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
         <v>106</v>
-      </c>
-      <c r="C28" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2092,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
         <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2103,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
         <v>114</v>
-      </c>
-      <c r="C30" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2114,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
         <v>118</v>
-      </c>
-      <c r="C31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2125,32 +2066,32 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
         <v>122</v>
-      </c>
-      <c r="C32" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
         <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
         <v>130</v>
-      </c>
-      <c r="C34" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2158,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
         <v>134</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2169,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2180,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2191,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
         <v>145</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2202,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
         <v>149</v>
-      </c>
-      <c r="C39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2213,10 +2154,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
         <v>153</v>
-      </c>
-      <c r="C40" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2224,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
         <v>157</v>
-      </c>
-      <c r="C41" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2235,10 +2176,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2246,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2261,36 +2202,6 @@
       </c>
       <c r="C44" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C47" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>